<commit_message>
Add image parse in excel_parser, add tests for image parsing
</commit_message>
<xml_diff>
--- a/tests/parsers/data/test_excel.xlsx
+++ b/tests/parsers/data/test_excel.xlsx
@@ -210,6 +210,87 @@
         <a:xfrm>
           <a:off x="609600" y="571500"/>
           <a:ext cx="9774014" cy="5439534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>596</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4267796" cy="1762371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>352815</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>181505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="2286000"/>
+          <a:ext cx="2791215" cy="3801005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1242,10 +1323,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make TODO, fix tests, add formulas parse
</commit_message>
<xml_diff>
--- a/tests/parsers/data/test_excel.xlsx
+++ b/tests/parsers/data/test_excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
     <sheet name="Лист6" sheetId="6" r:id="rId6"/>
+    <sheet name="Лист7" sheetId="7" r:id="rId7"/>
+    <sheet name="Лист8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1323,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
@@ -1332,4 +1334,61 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>SUM(C2,D3,E4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f>LOG10(B7)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>